<commit_message>
Updated the Data Driven User Tests along with other minor updates.
</commit_message>
<xml_diff>
--- a/testData/Userdata.xlsx
+++ b/testData/Userdata.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryan/Desktop/Learnings/Software Testing/API/AutomationFramework/FurStoreAutomation/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryan/Desktop/Learnings/Software Testing/API Testing/AutomationFramework/FurStoreAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{328301B4-8F1A-614F-B955-FB23913472CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A64738-A360-9A44-B00C-1A6895D6CA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1599D708-CC1A-714E-A874-B2C14CC5BB50}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{1599D708-CC1A-714E-A874-B2C14CC5BB50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -95,20 +96,38 @@
     <t>Bobby</t>
   </si>
   <si>
-    <t>testuser1</t>
-  </si>
-  <si>
-    <t>testuser2</t>
-  </si>
-  <si>
-    <t>testuser3</t>
+    <t>BobbyUpdated</t>
+  </si>
+  <si>
+    <t>HoneyUpdated</t>
+  </si>
+  <si>
+    <t>updated_a@gmail.com</t>
+  </si>
+  <si>
+    <t>updated_b@gmail.com</t>
+  </si>
+  <si>
+    <t>updated_c@gmail.com</t>
+  </si>
+  <si>
+    <t>user_1</t>
+  </si>
+  <si>
+    <t>user_2</t>
+  </si>
+  <si>
+    <t>user_3</t>
+  </si>
+  <si>
+    <t>AkashUpdated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,6 +139,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -486,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B792C-D52D-794D-894B-9E7199156160}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +548,7 @@
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -546,7 +571,7 @@
         <v>1002</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -569,7 +594,7 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -595,4 +620,121 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A97A88-1714-0644-A0EC-DDB95A8F1659}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{10B4075C-7A01-5F40-A7BF-2E423AB1EAA7}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{84802DCA-26F9-9C45-97F9-37C44432713B}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{62E26B12-5D5F-2C4F-BB49-96964339954E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>